<commit_message>
change age to birthDate on person class
</commit_message>
<xml_diff>
--- a/src/main/resources/students-template.xlsx
+++ b/src/main/resources/students-template.xlsx
@@ -35,7 +35,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">:page
-7
+9
 5</t>
         </r>
       </text>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Age</t>
+    <t xml:space="preserve">Birth Date</t>
   </si>
   <si>
     <t xml:space="preserve">Average Grade</t>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">It’s {name}</t>
   </si>
   <si>
-    <t xml:space="preserve">{age}</t>
+    <t xml:space="preserve">{birthDate|DATE}</t>
   </si>
   <si>
     <t xml:space="preserve">Living in {address}</t>
@@ -310,10 +310,10 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.88"/>

</xml_diff>